<commit_message>
Revision: Add Tutor Management and Exam History Features
</commit_message>
<xml_diff>
--- a/public/assets/excel/students.xlsx
+++ b/public/assets/excel/students.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LINTANG\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\JOKI\cbt-1\public\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1183CBED-CB0E-4620-ACC4-4D4CE84BE6BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2EA386-3BB9-4F16-84A3-BD16E45A7DE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{BF2F3F25-ADB9-4830-A867-F43D932DD398}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
-  <si>
-    <t>Nisn</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -73,6 +70,24 @@
   </si>
   <si>
     <t>08515831911</t>
+  </si>
+  <si>
+    <t>Nik</t>
+  </si>
+  <si>
+    <t>3518041000000001</t>
+  </si>
+  <si>
+    <t>3518041000000002</t>
+  </si>
+  <si>
+    <t>3518041000000003</t>
+  </si>
+  <si>
+    <t>3518041000000004</t>
+  </si>
+  <si>
+    <t>3518041000000005</t>
   </si>
 </sst>
 </file>
@@ -428,11 +443,12 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -441,137 +457,137 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>101</v>
+      <c r="A2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>102</v>
+      <c r="A3" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>103</v>
+      <c r="A4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>104</v>
+      <c r="A5" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>105</v>
+      <c r="A6" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
       </c>
       <c r="G6">
         <v>1</v>

</xml_diff>